<commit_message>
Alterando nome das variáveis
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,11 +484,6 @@
           <t>Estado</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>CNPJ:</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -542,7 +537,6 @@
           <t>Bahia</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -598,7 +592,6 @@
           <t>Bahia</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -654,7 +647,6 @@
           <t>Bahia</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -704,11 +696,6 @@
         </is>
       </c>
       <c r="J5" t="inlineStr">
-        <is>
-          <t>Bahia</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
         <is>
           <t>46042299000148 - Sócio Pessoa Jurídica Domiciliado no Exterior (Estados Unidos) Representado por Roberto Lazaro dos Santos - Procurador
 Roberto Lazaro dos Santos - Sócio-Administrador</t>
@@ -771,7 +758,6 @@
           <t>Bahia</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -827,12 +813,6 @@
           <t>Bahia</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>25526407000188 - Sócio Representado por Ossami Sakamori - Administrador
-Luiz Humberto Menezes Portugal de Lima - Sócio-Administrador</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -888,7 +868,6 @@
           <t>Bahia</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>